<commit_message>
we have strike a nerve
</commit_message>
<xml_diff>
--- a/task/TOP_TARGETS.xlsx
+++ b/task/TOP_TARGETS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ad0791/Desktop/Hanwash.mwater.dev/task/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{808C2447-6D8A-5C43-A50E-884B582300F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06220231-557C-0146-9AD7-E8A44F0B1B8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="3" xr2:uid="{EC7AEB5B-A1BD-6F43-A7A1-7D858BCB7C93}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{EC7AEB5B-A1BD-6F43-A7A1-7D858BCB7C93}"/>
   </bookViews>
   <sheets>
     <sheet name="leaders_commitees" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,12 @@
     <sheet name="hanwash_ambassadors" sheetId="3" r:id="rId3"/>
     <sheet name="Project_teams" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">hanwash_ambassadors!$A$1:$F$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">leaders_commitees!$A$1:$E$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Project_teams!$A$1:$E$14</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'staff consultant'!$A$1:$E$8</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -38,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="148">
   <si>
     <t>Deborah</t>
   </si>
@@ -116,9 +122,6 @@
   </si>
   <si>
     <t>Haiti Liaison Secretary</t>
-  </si>
-  <si>
-    <t>nixon.sem@hanwash.org</t>
   </si>
   <si>
     <t>Andre</t>
@@ -515,6 +518,18 @@
   </si>
   <si>
     <t>dantilplus@gmail.com</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>outlook</t>
+  </si>
+  <si>
+    <t>nixon.seme@hanwash.org</t>
+  </si>
+  <si>
+    <t>outloook</t>
   </si>
 </sst>
 </file>
@@ -614,24 +629,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -948,285 +960,301 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E82BFB58-FADC-334D-B6FD-5B05560C3B07}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="31.33203125" customWidth="1"/>
-    <col min="3" max="3" width="40" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.33203125" customWidth="1"/>
     <col min="4" max="4" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" hidden="1">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="6" t="s">
+    <row r="4" spans="1:5" hidden="1">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" hidden="1">
+      <c r="A5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" hidden="1">
+      <c r="A7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" hidden="1">
+      <c r="A8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" hidden="1">
+      <c r="A9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" hidden="1">
+      <c r="A12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" hidden="1">
+      <c r="A13" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" hidden="1">
+      <c r="A15" s="5" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D14" s="5" t="s">
+      <c r="B15" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E14" s="6" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="B15" s="7" t="s">
+      <c r="D15" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D15" s="8"/>
-      <c r="E15" s="6"/>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="7" t="s">
+      <c r="B16" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B16" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="6"/>
+      <c r="C16" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>140</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E16" xr:uid="{E82BFB58-FADC-334D-B6FD-5B05560C3B07}">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="NO"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" tooltip="mailto:deborahyhowell7020@gmail.com" display="mailto:deborahyhowell7020@gmail.com" xr:uid="{E99857B2-6B2C-3E48-9318-9209BFD647D4}"/>
     <hyperlink ref="D3" r:id="rId2" tooltip="mailto:lindseycancino@gmail.com" display="mailto:lindseycancino@gmail.com" xr:uid="{69F7E1E5-FE79-134A-B721-EA01DC483500}"/>
@@ -1234,7 +1262,7 @@
     <hyperlink ref="D5" r:id="rId4" tooltip="mailto:RotarianBob@hometownu.biz" display="mailto:RotarianBob@hometownu.biz" xr:uid="{BF7D7B8A-B383-344A-B6BE-A60675C28810}"/>
     <hyperlink ref="D6" r:id="rId5" tooltip="mailto:dale@haitioutreach.org" display="mailto:dale@haitioutreach.org" xr:uid="{885B5F75-513B-3E43-8876-A2F34FDDB10E}"/>
     <hyperlink ref="D7" r:id="rId6" tooltip="mailto:mgay@cfetsa.com" display="mailto:mgay@cfetsa.com" xr:uid="{8913A809-2481-8A43-9B13-C0AD2AF030AE}"/>
-    <hyperlink ref="D8" r:id="rId7" tooltip="mailto:nixon.sem@hanwash.org" display="mailto:nixon.sem@hanwash.org" xr:uid="{4D0B6C34-3E69-0643-9ED0-FE3CC99281C3}"/>
+    <hyperlink ref="D8" r:id="rId7" xr:uid="{4D0B6C34-3E69-0643-9ED0-FE3CC99281C3}"/>
     <hyperlink ref="D9" r:id="rId8" tooltip="mailto:andrewildaine@gmail.com" display="mailto:andrewildaine@gmail.com" xr:uid="{E0C549F6-DBB1-EB41-8141-3A034D91267A}"/>
     <hyperlink ref="D10" r:id="rId9" tooltip="mailto:sue@goldsen.com" display="mailto:sue@goldsen.com" xr:uid="{9E6B5964-F9FB-F441-A82F-F4036C709FA6}"/>
     <hyperlink ref="D11" r:id="rId10" tooltip="mailto:terrym@ridistrict6290.org" display="mailto:terrym@ridistrict6290.org" xr:uid="{A5D824B1-E852-4D46-869D-20D1280BAB97}"/>
@@ -1248,10 +1276,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C8EFA09-7872-5F4B-93DB-214017F34D64}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="18.83203125" defaultRowHeight="16"/>
@@ -1260,130 +1289,137 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B1" s="3" t="s">
+      <c r="A1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" hidden="1">
+      <c r="A2" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="B2" s="6" t="s">
+      <c r="C2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" hidden="1">
+      <c r="A3" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="6" t="s">
+      <c r="B3" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="C3" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" hidden="1">
+      <c r="A4" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="6" t="s">
+      <c r="B4" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="C4" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="6" t="s">
+      <c r="B5" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="C5" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" hidden="1">
+      <c r="A6" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="6" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="6" t="s">
+      <c r="B6" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="C6" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="D6" s="7"/>
+      <c r="E6" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" hidden="1">
+      <c r="A7" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="D6" s="13"/>
-      <c r="E6" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="6" t="s">
+      <c r="B7" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="C7" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D7" s="7"/>
+      <c r="E7" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="D7" s="13"/>
-      <c r="E7" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="6" t="s">
-        <v>141</v>
+      <c r="C8" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" s="7"/>
+      <c r="E8" s="4" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E8" xr:uid="{2C8EFA09-7872-5F4B-93DB-214017F34D64}">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="NO"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="1">
     <mergeCell ref="D2:D8"/>
   </mergeCells>
@@ -1393,10 +1429,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9ACD411-58AB-3947-A3EB-DCD200358794}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="E4" sqref="E4:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1410,126 +1447,133 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="C1" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="E1" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="F1" s="9" t="s">
+    </row>
+    <row r="2" spans="1:6" hidden="1">
+      <c r="A2" s="9" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="C2" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="D2" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="E2" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" hidden="1">
+      <c r="A3" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="E2" t="s">
+      <c r="B3" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" hidden="1">
+      <c r="A5" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="F2" s="10" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="D4" t="s">
-        <v>97</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>141</v>
+      <c r="F6" s="9" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F6" xr:uid="{A9ACD411-58AB-3947-A3EB-DCD200358794}">
+    <filterColumn colId="5">
+      <filters>
+        <filter val="NO"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <hyperlinks>
     <hyperlink ref="E6" r:id="rId1" tooltip="mailto:fritz.pierrelouis@hanwash.org" display="mailto:fritz.pierrelouis@hanwash.org" xr:uid="{C42B1722-17AE-994B-846F-B3DCF5F2D108}"/>
     <hyperlink ref="E3" r:id="rId2" tooltip="mailto:alcenate@yahoo.fr" display="mailto:alcenate@yahoo.fr" xr:uid="{0710B1B1-E780-794C-A9E4-5595AAA378B3}"/>
@@ -1542,10 +1586,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6259A1DC-D140-7C4B-AEDA-60CA72DE433C}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1558,211 +1603,229 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="28" customHeight="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="E1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" hidden="1">
+      <c r="A4" s="4" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B2" t="s">
-        <v>116</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="B4" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" hidden="1">
+      <c r="A6" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="D11" s="8" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="E3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>114</v>
-      </c>
-      <c r="B4" t="s">
-        <v>125</v>
-      </c>
-      <c r="D4" t="s">
-        <v>126</v>
-      </c>
-      <c r="E4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>114</v>
-      </c>
-      <c r="B5" t="s">
-        <v>127</v>
-      </c>
-      <c r="D5" t="s">
-        <v>128</v>
-      </c>
-      <c r="E5" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>115</v>
-      </c>
-      <c r="B6" t="s">
-        <v>120</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="E6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>115</v>
-      </c>
-      <c r="B7" t="s">
-        <v>123</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="E7" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
-        <v>115</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="E8" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
-        <v>115</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="E9" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
-        <v>96</v>
-      </c>
-      <c r="B10" t="s">
-        <v>129</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E10" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" t="s">
-        <v>96</v>
-      </c>
-      <c r="B11" t="s">
-        <v>130</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="E11" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B12" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="D11" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="E11" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" t="s">
-        <v>95</v>
-      </c>
-      <c r="B12" s="10" t="s">
+      <c r="C12" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="D12" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D12" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="E12" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" t="s">
-        <v>95</v>
-      </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="4"/>
+      <c r="D13" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="E13" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E13" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" t="s">
-        <v>95</v>
-      </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="4"/>
+      <c r="D14" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="E14" t="s">
-        <v>141</v>
+      <c r="E14" s="4" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E14" xr:uid="{6259A1DC-D140-7C4B-AEDA-60CA72DE433C}">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="NO"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <hyperlinks>
     <hyperlink ref="D10" r:id="rId1" tooltip="mailto:sherry@adobie.com" display="mailto:sherry@adobie.com" xr:uid="{2F2738DB-A5DC-C841-B166-687FCF6C1562}"/>
     <hyperlink ref="D13" r:id="rId2" xr:uid="{1784C06B-B663-A34E-832D-5B5F9F581A9B}"/>

</xml_diff>

<commit_message>
we made a push
</commit_message>
<xml_diff>
--- a/task/TOP_TARGETS.xlsx
+++ b/task/TOP_TARGETS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ad0791/Desktop/Hanwash.mwater.dev/task/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46D980A9-4FFC-E54A-830C-F6D5E88CA9D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E521AD22-EC5C-5643-96CD-8EFCE031D8C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{EC7AEB5B-A1BD-6F43-A7A1-7D858BCB7C93}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="3" xr2:uid="{EC7AEB5B-A1BD-6F43-A7A1-7D858BCB7C93}"/>
   </bookViews>
   <sheets>
     <sheet name="leaders_commitees" sheetId="1" r:id="rId1"/>
@@ -978,8 +978,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1160,7 +1160,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" hidden="1">
       <c r="A11" s="2" t="s">
         <v>34</v>
       </c>
@@ -1174,7 +1174,7 @@
         <v>37</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>139</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:5" hidden="1">
@@ -1447,7 +1447,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1603,8 +1603,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>